<commit_message>
Update Excel files for Hutschienenmoped-XL.
</commit_message>
<xml_diff>
--- a/Hutschienenmoped-XL/JLCSMT_Sample_CPL1.xlsx
+++ b/Hutschienenmoped-XL/JLCSMT_Sample_CPL1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ms\ISOBUS_Hardware\Hutschienenmoped-XL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A243A7-6C0B-4406-AF89-80B66AA05EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3ABE5FF-93A0-4374-AE93-6B706AA82BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42255" yWindow="1440" windowWidth="33435" windowHeight="18735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5970" yWindow="1470" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="132">
   <si>
     <t>Designator</t>
   </si>
@@ -362,6 +362,60 @@
   </si>
   <si>
     <t>U6</t>
+  </si>
+  <si>
+    <t>D014</t>
+  </si>
+  <si>
+    <t>D016</t>
+  </si>
+  <si>
+    <t>D018</t>
+  </si>
+  <si>
+    <t>D019</t>
+  </si>
+  <si>
+    <t>D020</t>
+  </si>
+  <si>
+    <t>D021</t>
+  </si>
+  <si>
+    <t>D022</t>
+  </si>
+  <si>
+    <t>D023</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>R34</t>
+  </si>
+  <si>
+    <t>R35</t>
+  </si>
+  <si>
+    <t>R36</t>
+  </si>
+  <si>
+    <t>R37</t>
+  </si>
+  <si>
+    <t>R38</t>
   </si>
 </sst>
 </file>
@@ -719,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E109"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -810,7 +864,7 @@
         <v>38.1</v>
       </c>
       <c r="C5" s="3">
-        <v>21.61</v>
+        <v>23.74</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
@@ -861,7 +915,7 @@
         <v>17.78</v>
       </c>
       <c r="C8" s="3">
-        <v>21.61</v>
+        <v>23.74</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -878,7 +932,7 @@
         <v>27.94</v>
       </c>
       <c r="C9" s="3">
-        <v>21.61</v>
+        <v>23.74</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
@@ -895,7 +949,7 @@
         <v>48.26</v>
       </c>
       <c r="C10" s="3">
-        <v>21.61</v>
+        <v>23.74</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
@@ -963,7 +1017,7 @@
         <v>58.42</v>
       </c>
       <c r="C14" s="3">
-        <v>21.61</v>
+        <v>23.74</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
@@ -997,7 +1051,7 @@
         <v>68.58</v>
       </c>
       <c r="C16" s="3">
-        <v>21.61</v>
+        <v>23.74</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>6</v>
@@ -1082,7 +1136,7 @@
         <v>78.739999999999995</v>
       </c>
       <c r="C21" s="3">
-        <v>21.61</v>
+        <v>23.74</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>6</v>
@@ -1099,7 +1153,7 @@
         <v>88.9</v>
       </c>
       <c r="C22" s="3">
-        <v>21.61</v>
+        <v>23.74</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>6</v>
@@ -1637,27 +1691,27 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>59</v>
+        <v>114</v>
       </c>
       <c r="B54" s="3">
-        <v>27.94</v>
+        <v>17.78</v>
       </c>
       <c r="C54" s="3">
-        <v>60.96</v>
+        <v>21.15</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E54" s="3">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B55" s="3">
-        <v>38.1</v>
+        <v>27.94</v>
       </c>
       <c r="C55" s="3">
         <v>60.96</v>
@@ -1671,30 +1725,30 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="B56" s="3">
-        <v>82.09</v>
+        <v>38.1</v>
       </c>
       <c r="C56" s="3">
-        <v>63.96</v>
+        <v>21.15</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E56" s="3">
-        <v>135</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B57" s="3">
-        <v>80.84</v>
+        <v>38.1</v>
       </c>
       <c r="C57" s="3">
-        <v>82.28</v>
+        <v>60.96</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>6</v>
@@ -1705,149 +1759,149 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>9</v>
+        <v>116</v>
       </c>
       <c r="B58" s="3">
-        <v>44.48</v>
+        <v>48.26</v>
       </c>
       <c r="C58" s="3">
-        <v>35.119999999999997</v>
+        <v>21.15</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E58" s="3">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="B59" s="3">
-        <v>78.3</v>
+        <v>27.94</v>
       </c>
       <c r="C59" s="3">
-        <v>82.28</v>
+        <v>21.15</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E59" s="3">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="B60" s="3">
-        <v>41.88</v>
+        <v>58.42</v>
       </c>
       <c r="C60" s="3">
-        <v>35.119999999999997</v>
+        <v>21.15</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E60" s="3">
-        <v>270</v>
+        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="B61" s="3">
-        <v>64.8</v>
+        <v>68.58</v>
       </c>
       <c r="C61" s="3">
-        <v>35.119999999999997</v>
+        <v>21.15</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E61" s="3">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="B62" s="3">
-        <v>62.2</v>
+        <v>78.739999999999995</v>
       </c>
       <c r="C62" s="3">
-        <v>35.119999999999997</v>
+        <v>21.15</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E62" s="3">
-        <v>270</v>
+        <v>180</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="B63" s="3">
-        <v>34.29</v>
+        <v>88.9</v>
       </c>
       <c r="C63" s="3">
-        <v>40.659999999999997</v>
+        <v>21.15</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E63" s="3">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B64" s="3">
-        <v>67.31</v>
+        <v>82.09</v>
       </c>
       <c r="C64" s="3">
-        <v>40.659999999999997</v>
+        <v>63.96</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E64" s="3">
-        <v>270</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B65" s="3">
-        <v>85.12</v>
+        <v>80.84</v>
       </c>
       <c r="C65" s="3">
-        <v>35.119999999999997</v>
+        <v>82.28</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E65" s="3">
-        <v>270</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B66" s="3">
-        <v>26.67</v>
+        <v>44.48</v>
       </c>
       <c r="C66" s="3">
-        <v>40.659999999999997</v>
+        <v>35.119999999999997</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>6</v>
@@ -1858,30 +1912,30 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B67" s="3">
-        <v>82.52</v>
+        <v>78.3</v>
       </c>
       <c r="C67" s="3">
-        <v>35.119999999999997</v>
+        <v>82.28</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E67" s="3">
-        <v>270</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B68" s="3">
-        <v>74.930000000000007</v>
+        <v>41.88</v>
       </c>
       <c r="C68" s="3">
-        <v>40.659999999999997</v>
+        <v>35.119999999999997</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>6</v>
@@ -1892,10 +1946,10 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B69" s="3">
-        <v>21.56</v>
+        <v>64.8</v>
       </c>
       <c r="C69" s="3">
         <v>35.119999999999997</v>
@@ -1909,47 +1963,47 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B70" s="3">
-        <v>37.85</v>
+        <v>62.2</v>
       </c>
       <c r="C70" s="3">
-        <v>42.42</v>
+        <v>35.119999999999997</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E70" s="3">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B71" s="3">
-        <v>25.65</v>
+        <v>34.29</v>
       </c>
       <c r="C71" s="3">
-        <v>43.69</v>
+        <v>40.659999999999997</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E71" s="3">
-        <v>180</v>
+        <v>270</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B72" s="3">
-        <v>24.16</v>
+        <v>67.31</v>
       </c>
       <c r="C72" s="3">
-        <v>35.119999999999997</v>
+        <v>40.659999999999997</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>6</v>
@@ -1960,47 +2014,47 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B73" s="3">
-        <v>23.9</v>
+        <v>85.12</v>
       </c>
       <c r="C73" s="3">
-        <v>85.22</v>
+        <v>35.119999999999997</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E73" s="3">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B74" s="3">
-        <v>25.4</v>
+        <v>26.67</v>
       </c>
       <c r="C74" s="3">
-        <v>80.14</v>
+        <v>40.659999999999997</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E74" s="3">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B75" s="3">
-        <v>16.510000000000002</v>
+        <v>82.52</v>
       </c>
       <c r="C75" s="3">
-        <v>74.3</v>
+        <v>35.119999999999997</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>6</v>
@@ -2011,47 +2065,47 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B76" s="3">
-        <v>31.98</v>
+        <v>74.930000000000007</v>
       </c>
       <c r="C76" s="3">
-        <v>85.22</v>
+        <v>40.659999999999997</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E76" s="3">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B77" s="3">
-        <v>30.48</v>
+        <v>21.56</v>
       </c>
       <c r="C77" s="3">
-        <v>80.14</v>
+        <v>35.119999999999997</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E77" s="3">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B78" s="3">
-        <v>19.05</v>
+        <v>41.91</v>
       </c>
       <c r="C78" s="3">
-        <v>74.3</v>
+        <v>52.07</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>6</v>
@@ -2062,81 +2116,81 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B79" s="3">
-        <v>62.46</v>
+        <v>21.59</v>
       </c>
       <c r="C79" s="3">
-        <v>85.22</v>
+        <v>52.07</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E79" s="3">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>84</v>
+        <v>122</v>
       </c>
       <c r="B80" s="3">
-        <v>54.38</v>
+        <v>44.45</v>
       </c>
       <c r="C80" s="3">
-        <v>85.22</v>
+        <v>52.07</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E80" s="3">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="B81" s="3">
-        <v>60.96</v>
+        <v>46.99</v>
       </c>
       <c r="C81" s="3">
-        <v>80.14</v>
+        <v>52.07</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E81" s="3">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B82" s="3">
-        <v>55.88</v>
+        <v>24.16</v>
       </c>
       <c r="C82" s="3">
-        <v>80.14</v>
+        <v>35.119999999999997</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E82" s="3">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="B83" s="3">
         <v>49.53</v>
       </c>
       <c r="C83" s="3">
-        <v>74.3</v>
+        <v>52.07</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>6</v>
@@ -2147,13 +2201,13 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>88</v>
+        <v>125</v>
       </c>
       <c r="B84" s="3">
-        <v>46.99</v>
+        <v>60.96</v>
       </c>
       <c r="C84" s="3">
-        <v>74.3</v>
+        <v>52.07</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>6</v>
@@ -2164,10 +2218,10 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B85" s="3">
-        <v>34.06</v>
+        <v>23.9</v>
       </c>
       <c r="C85" s="3">
         <v>85.22</v>
@@ -2181,10 +2235,10 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B86" s="3">
-        <v>35.56</v>
+        <v>25.4</v>
       </c>
       <c r="C86" s="3">
         <v>80.14</v>
@@ -2198,10 +2252,10 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B87" s="3">
-        <v>26.67</v>
+        <v>16.510000000000002</v>
       </c>
       <c r="C87" s="3">
         <v>74.3</v>
@@ -2215,10 +2269,10 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B88" s="3">
-        <v>42.14</v>
+        <v>31.98</v>
       </c>
       <c r="C88" s="3">
         <v>85.22</v>
@@ -2232,10 +2286,10 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B89" s="3">
-        <v>40.64</v>
+        <v>30.48</v>
       </c>
       <c r="C89" s="3">
         <v>80.14</v>
@@ -2249,10 +2303,10 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B90" s="3">
-        <v>31.75</v>
+        <v>19.05</v>
       </c>
       <c r="C90" s="3">
         <v>74.3</v>
@@ -2266,10 +2320,10 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B91" s="3">
-        <v>44.22</v>
+        <v>62.46</v>
       </c>
       <c r="C91" s="3">
         <v>85.22</v>
@@ -2283,13 +2337,13 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B92" s="3">
-        <v>45.72</v>
+        <v>54.38</v>
       </c>
       <c r="C92" s="3">
-        <v>80.14</v>
+        <v>85.22</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>6</v>
@@ -2300,30 +2354,30 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B93" s="3">
-        <v>36.83</v>
+        <v>60.96</v>
       </c>
       <c r="C93" s="3">
-        <v>74.3</v>
+        <v>80.14</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E93" s="3">
-        <v>270</v>
+        <v>90</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B94" s="3">
-        <v>52.3</v>
+        <v>55.88</v>
       </c>
       <c r="C94" s="3">
-        <v>85.22</v>
+        <v>80.14</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>6</v>
@@ -2334,27 +2388,27 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B95" s="3">
-        <v>51.05</v>
+        <v>49.53</v>
       </c>
       <c r="C95" s="3">
-        <v>80.14</v>
+        <v>74.3</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E95" s="3">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B96" s="3">
-        <v>39.369999999999997</v>
+        <v>46.99</v>
       </c>
       <c r="C96" s="3">
         <v>74.3</v>
@@ -2368,30 +2422,30 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="B97" s="3">
-        <v>14.48</v>
+        <v>19.05</v>
       </c>
       <c r="C97" s="3">
-        <v>16.53</v>
+        <v>52.07</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E97" s="3">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="B98" s="3">
-        <v>31.24</v>
+        <v>58.42</v>
       </c>
       <c r="C98" s="3">
-        <v>16.53</v>
+        <v>52.07</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>6</v>
@@ -2402,30 +2456,30 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="B99" s="3">
-        <v>34.799999999999997</v>
+        <v>22.99</v>
       </c>
       <c r="C99" s="3">
-        <v>16.53</v>
+        <v>39.44</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E99" s="3">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="B100" s="3">
-        <v>51.31</v>
+        <v>43.18</v>
       </c>
       <c r="C100" s="3">
-        <v>16.53</v>
+        <v>39.44</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>6</v>
@@ -2436,13 +2490,13 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="B101" s="3">
-        <v>91.95</v>
+        <v>63.5</v>
       </c>
       <c r="C101" s="3">
-        <v>16.53</v>
+        <v>39.44</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>6</v>
@@ -2453,13 +2507,13 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="B102" s="3">
-        <v>71.88</v>
+        <v>80.56</v>
       </c>
       <c r="C102" s="3">
-        <v>16.53</v>
+        <v>39.44</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>6</v>
@@ -2470,13 +2524,13 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="B103" s="3">
-        <v>55.12</v>
+        <v>34.06</v>
       </c>
       <c r="C103" s="3">
-        <v>16.53</v>
+        <v>85.22</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>6</v>
@@ -2487,13 +2541,13 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="B104" s="3">
-        <v>75.44</v>
+        <v>35.56</v>
       </c>
       <c r="C104" s="3">
-        <v>16.53</v>
+        <v>80.14</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>6</v>
@@ -2504,13 +2558,13 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="B105" s="3">
-        <v>22.86</v>
+        <v>26.67</v>
       </c>
       <c r="C105" s="3">
-        <v>29.23</v>
+        <v>74.3</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>6</v>
@@ -2521,47 +2575,47 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="B106" s="3">
-        <v>43.18</v>
+        <v>42.14</v>
       </c>
       <c r="C106" s="3">
-        <v>29.23</v>
+        <v>85.22</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E106" s="3">
-        <v>270</v>
+        <v>90</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="B107" s="3">
-        <v>53.34</v>
+        <v>40.64</v>
       </c>
       <c r="C107" s="3">
-        <v>59.08</v>
+        <v>80.14</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E107" s="3">
-        <v>270</v>
+        <v>90</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="B108" s="3">
-        <v>63.5</v>
+        <v>31.75</v>
       </c>
       <c r="C108" s="3">
-        <v>29.23</v>
+        <v>74.3</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>6</v>
@@ -2572,18 +2626,324 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B109" s="3">
+        <v>44.22</v>
+      </c>
+      <c r="C109" s="3">
+        <v>85.22</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B110" s="3">
+        <v>45.72</v>
+      </c>
+      <c r="C110" s="3">
+        <v>80.14</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E110" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B111" s="3">
+        <v>36.83</v>
+      </c>
+      <c r="C111" s="3">
+        <v>74.3</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E111" s="3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B112" s="3">
+        <v>52.3</v>
+      </c>
+      <c r="C112" s="3">
+        <v>85.22</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E112" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B113" s="3">
+        <v>51.05</v>
+      </c>
+      <c r="C113" s="3">
+        <v>80.14</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E113" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B114" s="3">
+        <v>39.369999999999997</v>
+      </c>
+      <c r="C114" s="3">
+        <v>74.3</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E114" s="3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B115" s="3">
+        <v>14.48</v>
+      </c>
+      <c r="C115" s="3">
+        <v>16.53</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E115" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B116" s="3">
+        <v>31.24</v>
+      </c>
+      <c r="C116" s="3">
+        <v>16.53</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E116" s="3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B117" s="3">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="C117" s="3">
+        <v>16.53</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E117" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B118" s="3">
+        <v>51.31</v>
+      </c>
+      <c r="C118" s="3">
+        <v>16.53</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E118" s="3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B119" s="3">
+        <v>91.95</v>
+      </c>
+      <c r="C119" s="3">
+        <v>16.53</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E119" s="3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B120" s="3">
+        <v>71.88</v>
+      </c>
+      <c r="C120" s="3">
+        <v>16.53</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E120" s="3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B121" s="3">
+        <v>55.12</v>
+      </c>
+      <c r="C121" s="3">
+        <v>16.53</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E121" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B122" s="3">
+        <v>75.44</v>
+      </c>
+      <c r="C122" s="3">
+        <v>16.53</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E122" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B123" s="3">
+        <v>22.86</v>
+      </c>
+      <c r="C123" s="3">
+        <v>29.23</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E123" s="3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B124" s="3">
+        <v>43.18</v>
+      </c>
+      <c r="C124" s="3">
+        <v>29.23</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E124" s="3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B125" s="3">
+        <v>53.34</v>
+      </c>
+      <c r="C125" s="3">
+        <v>59.08</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E125" s="3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B126" s="3">
+        <v>63.5</v>
+      </c>
+      <c r="C126" s="3">
+        <v>29.23</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E126" s="3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B109" s="3">
+      <c r="B127" s="3">
         <v>83.82</v>
       </c>
-      <c r="C109" s="3">
+      <c r="C127" s="3">
         <v>29.23</v>
       </c>
-      <c r="D109" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E109" s="3">
+      <c r="D127" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E127" s="3">
         <v>270</v>
       </c>
     </row>

</xml_diff>